<commit_message>
new data from 23-24
</commit_message>
<xml_diff>
--- a/EU_PARK/europark_raw_files/Voletarium - Queue times in March 2024.xlsx
+++ b/EU_PARK/europark_raw_files/Voletarium - Queue times in March 2024.xlsx
@@ -4964,7 +4964,7 @@
     </row>
     <row r="571">
       <c r="A571" t="str">
-        <v>2024-03-16T12:31:00.000Z</v>
+        <v>2024-03-16T17:01:00.000Z</v>
       </c>
       <c r="B571" t="str">
         <v>N/A</v>
@@ -5212,7 +5212,7 @@
     </row>
     <row r="602">
       <c r="A602" t="str">
-        <v>2024-03-16T13:46:00.000Z</v>
+        <v>2024-03-16T18:16:00.000Z</v>
       </c>
       <c r="B602" t="str">
         <v>N/A</v>
@@ -10380,7 +10380,7 @@
     </row>
     <row r="1248">
       <c r="A1248" t="str">
-        <v>2024-03-17T13:46:00.000Z</v>
+        <v>2024-03-17T18:16:00.000Z</v>
       </c>
       <c r="B1248" t="str">
         <v>N/A</v>
@@ -10588,7 +10588,7 @@
     </row>
     <row r="1274">
       <c r="A1274" t="str">
-        <v>2024-03-23T03:52:00.000Z</v>
+        <v>2024-03-23T08:22:00.000Z</v>
       </c>
       <c r="B1274" t="str">
         <v>N/A</v>
@@ -10652,7 +10652,7 @@
     </row>
     <row r="1282">
       <c r="A1282" t="str">
-        <v>2024-03-23T04:00:00.000Z</v>
+        <v>2024-03-23T08:30:00.000Z</v>
       </c>
       <c r="B1282" t="str">
         <v>N/A</v>
@@ -10668,7 +10668,7 @@
     </row>
     <row r="1284">
       <c r="A1284" t="str">
-        <v>2024-03-23T04:03:00.000Z</v>
+        <v>2024-03-23T08:33:00.000Z</v>
       </c>
       <c r="B1284" t="str">
         <v>N/A</v>
@@ -10692,7 +10692,7 @@
     </row>
     <row r="1287">
       <c r="A1287" t="str">
-        <v>2024-03-23T04:28:00.000Z</v>
+        <v>2024-03-23T08:58:00.000Z</v>
       </c>
       <c r="B1287" t="str">
         <v>N/A</v>
@@ -10708,7 +10708,7 @@
     </row>
     <row r="1289">
       <c r="A1289" t="str">
-        <v>2024-03-23T04:46:00.000Z</v>
+        <v>2024-03-23T09:16:00.000Z</v>
       </c>
       <c r="B1289" t="str">
         <v>N/A</v>
@@ -10724,7 +10724,7 @@
     </row>
     <row r="1291">
       <c r="A1291" t="str">
-        <v>2024-03-23T04:55:00.000Z</v>
+        <v>2024-03-23T09:25:00.000Z</v>
       </c>
       <c r="B1291" t="str">
         <v>N/A</v>
@@ -10748,7 +10748,7 @@
     </row>
     <row r="1294">
       <c r="A1294" t="str">
-        <v>2024-03-23T05:00:00.000Z</v>
+        <v>2024-03-23T09:30:00.000Z</v>
       </c>
       <c r="B1294" t="str">
         <v>N/A</v>
@@ -10764,7 +10764,7 @@
     </row>
     <row r="1296">
       <c r="A1296" t="str">
-        <v>2024-03-23T05:02:00.000Z</v>
+        <v>2024-03-23T09:32:00.000Z</v>
       </c>
       <c r="B1296" t="str">
         <v>N/A</v>
@@ -10780,7 +10780,7 @@
     </row>
     <row r="1298">
       <c r="A1298" t="str">
-        <v>2024-03-23T05:04:00.000Z</v>
+        <v>2024-03-23T09:34:00.000Z</v>
       </c>
       <c r="B1298" t="str">
         <v>N/A</v>
@@ -10804,7 +10804,7 @@
     </row>
     <row r="1301">
       <c r="A1301" t="str">
-        <v>2024-03-23T05:14:00.000Z</v>
+        <v>2024-03-23T09:44:00.000Z</v>
       </c>
       <c r="B1301" t="str">
         <v>N/A</v>
@@ -10852,7 +10852,7 @@
     </row>
     <row r="1307">
       <c r="A1307" t="str">
-        <v>2024-03-23T05:22:00.000Z</v>
+        <v>2024-03-23T09:52:00.000Z</v>
       </c>
       <c r="B1307" t="str">
         <v>N/A</v>
@@ -10868,7 +10868,7 @@
     </row>
     <row r="1309">
       <c r="A1309" t="str">
-        <v>2024-03-23T05:24:00.000Z</v>
+        <v>2024-03-23T09:54:00.000Z</v>
       </c>
       <c r="B1309" t="str">
         <v>N/A</v>
@@ -10892,7 +10892,7 @@
     </row>
     <row r="1312">
       <c r="A1312" t="str">
-        <v>2024-03-23T05:28:00.000Z</v>
+        <v>2024-03-23T09:58:00.000Z</v>
       </c>
       <c r="B1312" t="str">
         <v>N/A</v>
@@ -11580,7 +11580,7 @@
     </row>
     <row r="1398">
       <c r="A1398" t="str">
-        <v>2024-03-23T06:56:00.000Z</v>
+        <v>2024-03-23T11:26:00.000Z</v>
       </c>
       <c r="B1398" t="str">
         <v>N/A</v>
@@ -11596,7 +11596,7 @@
     </row>
     <row r="1400">
       <c r="A1400" t="str">
-        <v>2024-03-23T06:58:00.000Z</v>
+        <v>2024-03-23T11:28:00.000Z</v>
       </c>
       <c r="B1400" t="str">
         <v>N/A</v>
@@ -11612,7 +11612,7 @@
     </row>
     <row r="1402">
       <c r="A1402" t="str">
-        <v>2024-03-23T07:00:00.000Z</v>
+        <v>2024-03-23T11:30:00.000Z</v>
       </c>
       <c r="B1402" t="str">
         <v>N/A</v>
@@ -11636,7 +11636,7 @@
     </row>
     <row r="1405">
       <c r="A1405" t="str">
-        <v>2024-03-23T07:03:00.000Z</v>
+        <v>2024-03-23T11:33:00.000Z</v>
       </c>
       <c r="B1405" t="str">
         <v>N/A</v>
@@ -11660,7 +11660,7 @@
     </row>
     <row r="1408">
       <c r="A1408" t="str">
-        <v>2024-03-23T07:08:00.000Z</v>
+        <v>2024-03-23T11:38:00.000Z</v>
       </c>
       <c r="B1408" t="str">
         <v>N/A</v>
@@ -11796,7 +11796,7 @@
     </row>
     <row r="1425">
       <c r="A1425" t="str">
-        <v>2024-03-23T07:26:00.000Z</v>
+        <v>2024-03-23T11:56:00.000Z</v>
       </c>
       <c r="B1425" t="str">
         <v>N/A</v>
@@ -11876,7 +11876,7 @@
     </row>
     <row r="1435">
       <c r="A1435" t="str">
-        <v>2024-03-23T07:36:00.000Z</v>
+        <v>2024-03-23T12:06:00.000Z</v>
       </c>
       <c r="B1435" t="str">
         <v>N/A</v>
@@ -11892,7 +11892,7 @@
     </row>
     <row r="1437">
       <c r="A1437" t="str">
-        <v>2024-03-23T07:40:00.000Z</v>
+        <v>2024-03-23T12:10:00.000Z</v>
       </c>
       <c r="B1437" t="str">
         <v>N/A</v>
@@ -11908,7 +11908,7 @@
     </row>
     <row r="1439">
       <c r="A1439" t="str">
-        <v>2024-03-23T07:43:00.000Z</v>
+        <v>2024-03-23T12:13:00.000Z</v>
       </c>
       <c r="B1439" t="str">
         <v>N/A</v>
@@ -11940,7 +11940,7 @@
     </row>
     <row r="1443">
       <c r="A1443" t="str">
-        <v>2024-03-23T07:48:00.000Z</v>
+        <v>2024-03-23T12:18:00.000Z</v>
       </c>
       <c r="B1443" t="str">
         <v>N/A</v>
@@ -11980,7 +11980,7 @@
     </row>
     <row r="1448">
       <c r="A1448" t="str">
-        <v>2024-03-23T07:58:00.000Z</v>
+        <v>2024-03-23T12:28:00.000Z</v>
       </c>
       <c r="B1448" t="str">
         <v>N/A</v>
@@ -12052,7 +12052,7 @@
     </row>
     <row r="1457">
       <c r="A1457" t="str">
-        <v>2024-03-23T08:07:00.000Z</v>
+        <v>2024-03-23T12:37:00.000Z</v>
       </c>
       <c r="B1457" t="str">
         <v>N/A</v>
@@ -12164,7 +12164,7 @@
     </row>
     <row r="1471">
       <c r="A1471" t="str">
-        <v>2024-03-23T08:21:00.000Z</v>
+        <v>2024-03-23T12:51:00.000Z</v>
       </c>
       <c r="B1471" t="str">
         <v>N/A</v>
@@ -12204,7 +12204,7 @@
     </row>
     <row r="1476">
       <c r="A1476" t="str">
-        <v>2024-03-23T08:26:00.000Z</v>
+        <v>2024-03-23T12:56:00.000Z</v>
       </c>
       <c r="B1476" t="str">
         <v>N/A</v>
@@ -12228,7 +12228,7 @@
     </row>
     <row r="1479">
       <c r="A1479" t="str">
-        <v>2024-03-23T08:40:00.000Z</v>
+        <v>2024-03-23T13:10:00.000Z</v>
       </c>
       <c r="B1479" t="str">
         <v>N/A</v>
@@ -12308,7 +12308,7 @@
     </row>
     <row r="1489">
       <c r="A1489" t="str">
-        <v>2024-03-23T08:51:00.000Z</v>
+        <v>2024-03-23T13:21:00.000Z</v>
       </c>
       <c r="B1489" t="str">
         <v>N/A</v>
@@ -12388,7 +12388,7 @@
     </row>
     <row r="1499">
       <c r="A1499" t="str">
-        <v>2024-03-23T09:01:00.000Z</v>
+        <v>2024-03-23T13:31:00.000Z</v>
       </c>
       <c r="B1499" t="str">
         <v>N/A</v>
@@ -12492,7 +12492,7 @@
     </row>
     <row r="1512">
       <c r="A1512" t="str">
-        <v>2024-03-23T09:14:00.000Z</v>
+        <v>2024-03-23T13:44:00.000Z</v>
       </c>
       <c r="B1512" t="str">
         <v>N/A</v>
@@ -12524,7 +12524,7 @@
     </row>
     <row r="1516">
       <c r="A1516" t="str">
-        <v>2024-03-23T09:19:00.000Z</v>
+        <v>2024-03-23T13:49:00.000Z</v>
       </c>
       <c r="B1516" t="str">
         <v>N/A</v>
@@ -14660,7 +14660,7 @@
     </row>
     <row r="1783">
       <c r="A1783" t="str">
-        <v>2024-03-23T13:46:00.000Z</v>
+        <v>2024-03-23T18:16:00.000Z</v>
       </c>
       <c r="B1783" t="str">
         <v>N/A</v>
@@ -19868,7 +19868,7 @@
     </row>
     <row r="2434">
       <c r="A2434" t="str">
-        <v>2024-03-24T13:46:00.000Z</v>
+        <v>2024-03-24T18:16:00.000Z</v>
       </c>
       <c r="B2434" t="str">
         <v>N/A</v>
@@ -24860,7 +24860,7 @@
     </row>
     <row r="3058">
       <c r="A3058" t="str">
-        <v>2024-03-25T13:16:00.000Z</v>
+        <v>2024-03-25T17:46:00.000Z</v>
       </c>
       <c r="B3058" t="str">
         <v>N/A</v>
@@ -29756,7 +29756,7 @@
     </row>
     <row r="3670">
       <c r="A3670" t="str">
-        <v>2024-03-26T13:16:00.000Z</v>
+        <v>2024-03-26T17:46:00.000Z</v>
       </c>
       <c r="B3670" t="str">
         <v>N/A</v>
@@ -34796,7 +34796,7 @@
     </row>
     <row r="4300">
       <c r="A4300" t="str">
-        <v>2024-03-27T13:16:00.000Z</v>
+        <v>2024-03-27T17:46:00.000Z</v>
       </c>
       <c r="B4300" t="str">
         <v>N/A</v>
@@ -39796,7 +39796,7 @@
     </row>
     <row r="4925">
       <c r="A4925" t="str">
-        <v>2024-03-28T13:16:00.000Z</v>
+        <v>2024-03-28T17:46:00.000Z</v>
       </c>
       <c r="B4925" t="str">
         <v>N/A</v>
@@ -44996,7 +44996,7 @@
     </row>
     <row r="5575">
       <c r="A5575" t="str">
-        <v>2024-03-29T13:46:00.000Z</v>
+        <v>2024-03-29T18:16:00.000Z</v>
       </c>
       <c r="B5575" t="str">
         <v>N/A</v>
@@ -45612,7 +45612,7 @@
     </row>
     <row r="5652">
       <c r="A5652" t="str">
-        <v>2024-03-30T04:15:00.000Z</v>
+        <v>2024-03-30T08:45:00.000Z</v>
       </c>
       <c r="B5652" t="str">
         <v>N/A</v>
@@ -45636,7 +45636,7 @@
     </row>
     <row r="5655">
       <c r="A5655" t="str">
-        <v>2024-03-30T04:19:00.000Z</v>
+        <v>2024-03-30T08:49:00.000Z</v>
       </c>
       <c r="B5655" t="str">
         <v>N/A</v>
@@ -45652,7 +45652,7 @@
     </row>
     <row r="5657">
       <c r="A5657" t="str">
-        <v>2024-03-30T04:33:00.000Z</v>
+        <v>2024-03-30T09:03:00.000Z</v>
       </c>
       <c r="B5657" t="str">
         <v>N/A</v>
@@ -45692,7 +45692,7 @@
     </row>
     <row r="5662">
       <c r="A5662" t="str">
-        <v>2024-03-30T04:47:00.000Z</v>
+        <v>2024-03-30T09:17:00.000Z</v>
       </c>
       <c r="B5662" t="str">
         <v>N/A</v>
@@ -45708,7 +45708,7 @@
     </row>
     <row r="5664">
       <c r="A5664" t="str">
-        <v>2024-03-30T04:50:00.000Z</v>
+        <v>2024-03-30T09:20:00.000Z</v>
       </c>
       <c r="B5664" t="str">
         <v>N/A</v>
@@ -45724,7 +45724,7 @@
     </row>
     <row r="5666">
       <c r="A5666" t="str">
-        <v>2024-03-30T04:54:00.000Z</v>
+        <v>2024-03-30T09:24:00.000Z</v>
       </c>
       <c r="B5666" t="str">
         <v>N/A</v>
@@ -45764,7 +45764,7 @@
     </row>
     <row r="5671">
       <c r="A5671" t="str">
-        <v>2024-03-30T05:00:00.000Z</v>
+        <v>2024-03-30T09:30:00.000Z</v>
       </c>
       <c r="B5671" t="str">
         <v>N/A</v>
@@ -45788,7 +45788,7 @@
     </row>
     <row r="5674">
       <c r="A5674" t="str">
-        <v>2024-03-30T05:15:00.000Z</v>
+        <v>2024-03-30T09:45:00.000Z</v>
       </c>
       <c r="B5674" t="str">
         <v>N/A</v>
@@ -45804,7 +45804,7 @@
     </row>
     <row r="5676">
       <c r="A5676" t="str">
-        <v>2024-03-30T05:29:00.000Z</v>
+        <v>2024-03-30T09:59:00.000Z</v>
       </c>
       <c r="B5676" t="str">
         <v>N/A</v>
@@ -45836,7 +45836,7 @@
     </row>
     <row r="5680">
       <c r="A5680" t="str">
-        <v>2024-03-30T05:34:00.000Z</v>
+        <v>2024-03-30T10:04:00.000Z</v>
       </c>
       <c r="B5680" t="str">
         <v>N/A</v>
@@ -46020,7 +46020,7 @@
     </row>
     <row r="5703">
       <c r="A5703" t="str">
-        <v>2024-03-30T05:59:00.000Z</v>
+        <v>2024-03-30T10:29:00.000Z</v>
       </c>
       <c r="B5703" t="str">
         <v>N/A</v>
@@ -46052,7 +46052,7 @@
     </row>
     <row r="5707">
       <c r="A5707" t="str">
-        <v>2024-03-30T06:04:00.000Z</v>
+        <v>2024-03-30T10:34:00.000Z</v>
       </c>
       <c r="B5707" t="str">
         <v>N/A</v>
@@ -46108,7 +46108,7 @@
     </row>
     <row r="5714">
       <c r="A5714" t="str">
-        <v>2024-03-30T06:12:00.000Z</v>
+        <v>2024-03-30T10:42:00.000Z</v>
       </c>
       <c r="B5714" t="str">
         <v>N/A</v>
@@ -46124,7 +46124,7 @@
     </row>
     <row r="5716">
       <c r="A5716" t="str">
-        <v>2024-03-30T06:15:00.000Z</v>
+        <v>2024-03-30T10:45:00.000Z</v>
       </c>
       <c r="B5716" t="str">
         <v>N/A</v>
@@ -46140,7 +46140,7 @@
     </row>
     <row r="5718">
       <c r="A5718" t="str">
-        <v>2024-03-30T06:28:00.000Z</v>
+        <v>2024-03-30T10:58:00.000Z</v>
       </c>
       <c r="B5718" t="str">
         <v>N/A</v>
@@ -46468,7 +46468,7 @@
     </row>
     <row r="5759">
       <c r="A5759" t="str">
-        <v>2024-03-30T07:10:00.000Z</v>
+        <v>2024-03-30T11:40:00.000Z</v>
       </c>
       <c r="B5759" t="str">
         <v>N/A</v>
@@ -46572,7 +46572,7 @@
     </row>
     <row r="5772">
       <c r="A5772" t="str">
-        <v>2024-03-30T07:24:00.000Z</v>
+        <v>2024-03-30T11:54:00.000Z</v>
       </c>
       <c r="B5772" t="str">
         <v>N/A</v>
@@ -46596,7 +46596,7 @@
     </row>
     <row r="5775">
       <c r="A5775" t="str">
-        <v>2024-03-30T07:27:00.000Z</v>
+        <v>2024-03-30T11:57:00.000Z</v>
       </c>
       <c r="B5775" t="str">
         <v>N/A</v>
@@ -46612,7 +46612,7 @@
     </row>
     <row r="5777">
       <c r="A5777" t="str">
-        <v>2024-03-30T07:30:00.000Z</v>
+        <v>2024-03-30T12:00:00.000Z</v>
       </c>
       <c r="B5777" t="str">
         <v>N/A</v>
@@ -46628,7 +46628,7 @@
     </row>
     <row r="5779">
       <c r="A5779" t="str">
-        <v>2024-03-30T07:35:00.000Z</v>
+        <v>2024-03-30T12:05:00.000Z</v>
       </c>
       <c r="B5779" t="str">
         <v>N/A</v>
@@ -46708,7 +46708,7 @@
     </row>
     <row r="5789">
       <c r="A5789" t="str">
-        <v>2024-03-30T07:46:00.000Z</v>
+        <v>2024-03-30T12:16:00.000Z</v>
       </c>
       <c r="B5789" t="str">
         <v>N/A</v>
@@ -46756,7 +46756,7 @@
     </row>
     <row r="5795">
       <c r="A5795" t="str">
-        <v>2024-03-30T07:53:00.000Z</v>
+        <v>2024-03-30T12:23:00.000Z</v>
       </c>
       <c r="B5795" t="str">
         <v>N/A</v>
@@ -46812,7 +46812,7 @@
     </row>
     <row r="5802">
       <c r="A5802" t="str">
-        <v>2024-03-30T08:01:00.000Z</v>
+        <v>2024-03-30T12:31:00.000Z</v>
       </c>
       <c r="B5802" t="str">
         <v>N/A</v>
@@ -46844,7 +46844,7 @@
     </row>
     <row r="5806">
       <c r="A5806" t="str">
-        <v>2024-03-30T08:07:00.000Z</v>
+        <v>2024-03-30T12:37:00.000Z</v>
       </c>
       <c r="B5806" t="str">
         <v>N/A</v>
@@ -46868,7 +46868,7 @@
     </row>
     <row r="5809">
       <c r="A5809" t="str">
-        <v>2024-03-30T08:13:00.000Z</v>
+        <v>2024-03-30T12:43:00.000Z</v>
       </c>
       <c r="B5809" t="str">
         <v>N/A</v>
@@ -46884,7 +46884,7 @@
     </row>
     <row r="5811">
       <c r="A5811" t="str">
-        <v>2024-03-30T08:16:00.000Z</v>
+        <v>2024-03-30T12:46:00.000Z</v>
       </c>
       <c r="B5811" t="str">
         <v>N/A</v>
@@ -46916,7 +46916,7 @@
     </row>
     <row r="5815">
       <c r="A5815" t="str">
-        <v>2024-03-30T08:21:00.000Z</v>
+        <v>2024-03-30T12:51:00.000Z</v>
       </c>
       <c r="B5815" t="str">
         <v>N/A</v>
@@ -46948,7 +46948,7 @@
     </row>
     <row r="5819">
       <c r="A5819" t="str">
-        <v>2024-03-30T08:26:00.000Z</v>
+        <v>2024-03-30T12:56:00.000Z</v>
       </c>
       <c r="B5819" t="str">
         <v>N/A</v>
@@ -46964,7 +46964,7 @@
     </row>
     <row r="5821">
       <c r="A5821" t="str">
-        <v>2024-03-30T08:29:00.000Z</v>
+        <v>2024-03-30T12:59:00.000Z</v>
       </c>
       <c r="B5821" t="str">
         <v>N/A</v>
@@ -46988,7 +46988,7 @@
     </row>
     <row r="5824">
       <c r="A5824" t="str">
-        <v>2024-03-30T08:35:00.000Z</v>
+        <v>2024-03-30T13:05:00.000Z</v>
       </c>
       <c r="B5824" t="str">
         <v>N/A</v>
@@ -47004,7 +47004,7 @@
     </row>
     <row r="5826">
       <c r="A5826" t="str">
-        <v>2024-03-30T08:40:00.000Z</v>
+        <v>2024-03-30T13:10:00.000Z</v>
       </c>
       <c r="B5826" t="str">
         <v>N/A</v>
@@ -47044,7 +47044,7 @@
     </row>
     <row r="5831">
       <c r="A5831" t="str">
-        <v>2024-03-30T08:48:00.000Z</v>
+        <v>2024-03-30T13:18:00.000Z</v>
       </c>
       <c r="B5831" t="str">
         <v>N/A</v>
@@ -47060,7 +47060,7 @@
     </row>
     <row r="5833">
       <c r="A5833" t="str">
-        <v>2024-03-30T08:54:00.000Z</v>
+        <v>2024-03-30T13:24:00.000Z</v>
       </c>
       <c r="B5833" t="str">
         <v>N/A</v>
@@ -49388,7 +49388,7 @@
     </row>
     <row r="6124">
       <c r="A6124" t="str">
-        <v>2024-03-30T13:46:00.000Z</v>
+        <v>2024-03-30T18:16:00.000Z</v>
       </c>
       <c r="B6124" t="str">
         <v>N/A</v>

</xml_diff>